<commit_message>
Se agregan los ultimos detalles al proyecto, como es el calculo de los precios
</commit_message>
<xml_diff>
--- a/Productos.xlsx
+++ b/Productos.xlsx
@@ -1,6 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr date1904="false"/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Nit</t>
   </si>
@@ -31,28 +32,34 @@
     <t>Precio Unitario</t>
   </si>
   <si>
-    <t>Precio Final</t>
-  </si>
-  <si>
-    <t>0901</t>
-  </si>
-  <si>
-    <t>Oliver</t>
-  </si>
-  <si>
-    <t>10107</t>
-  </si>
-  <si>
-    <t>Computadora</t>
-  </si>
-  <si>
-    <t>Jose</t>
-  </si>
-  <si>
-    <t>10108</t>
-  </si>
-  <si>
-    <t>Rasuradora</t>
+    <t>Precio Final sin iva</t>
+  </si>
+  <si>
+    <t>Precio final</t>
+  </si>
+  <si>
+    <t>888-8</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>Billetera</t>
+  </si>
+  <si>
+    <t>1234-5</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>2232</t>
+  </si>
+  <si>
+    <t>Mouse</t>
   </si>
 </sst>
 </file>
@@ -103,16 +110,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.41953125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="7.19921875"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.1240234375"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.2642578125"/>
+    <col min="1" max="1" width="7.28515625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="7.30078125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="7.2265625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="9.23828125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -137,51 +144,60 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="F2" t="n">
-        <v>5000.0</v>
+        <v>250.0</v>
       </c>
       <c r="G2" t="n">
-        <v>5000.0</v>
+        <v>669.643</v>
+      </c>
+      <c r="H2" t="n">
+        <v>750.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3" t="n">
         <v>2.0</v>
       </c>
       <c r="F3" t="n">
-        <v>10.0</v>
+        <v>250.0</v>
       </c>
       <c r="G3" t="n">
-        <v>20.0</v>
+        <v>446.429</v>
+      </c>
+      <c r="H3" t="n">
+        <v>500.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>